<commit_message>
Wrote a procedure for NOAA_Processor.R that is specific to the NOAA dataset (and independent of the Downsizer dataset)
</commit_message>
<xml_diff>
--- a/Supply/InputData/RR_PRMS_StationList (2023-09-05).xlsx
+++ b/Supply/InputData/RR_PRMS_StationList (2023-09-05).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26821"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards.sharepoint.com/DWR/SDA/Shared Documents/SOPs and Documentation/2. Hydro Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aprashar\Documents\Github\DWRAT_DataScraping\Supply\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A4A9023-C479-4456-BC78-957D045F84F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B09ED4D-E8B8-4597-B223-D8D958F73DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{55E5B8DA-EFB4-40EB-A996-34EBB2C6B909}"/>
   </bookViews>
   <sheets>
     <sheet name="StationList" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2841" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -45,6 +45,7 @@
     <author>tc={F7E1318F-72F2-47B4-98CD-48B1EDD3CC0B}</author>
     <author>tc={DC39DFA2-B6F7-4426-AEFC-0E29DFA05EC6}</author>
     <author>tc={AD3D0412-D381-472E-8164-396C8D02E097}</author>
+    <author>tc={42A02FD6-F123-4517-A0FF-D7A041A3BB47}</author>
     <author>tc={67604B43-B0E8-4EFB-8E4E-E4BE87F04D43}</author>
     <author>tc={CCF7D895-9024-4EB3-B4C8-9D4267AD910D}</author>
     <author>tc={CCE18EB5-1980-4F82-8A29-0E47102B130E}</author>
@@ -117,7 +118,15 @@
     The PRISM stations that are used to fill in the missing data for our weather stations have the same longitude and latitude, but different elevations. Is this an issue?</t>
       </text>
     </comment>
-    <comment ref="H3" authorId="6" shapeId="0" xr:uid="{67604B43-B0E8-4EFB-8E4E-E4BE87F04D43}">
+    <comment ref="A3" authorId="6" shapeId="0" xr:uid="{42A02FD6-F123-4517-A0FF-D7A041A3BB47}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NOAA stations were formerly DOWNSIZER stations, but then SDU discovered that the program Downsizer is a GUI for collecting NOAA station data. Hence, we decided to download data from NOAA directly instead. </t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="7" shapeId="0" xr:uid="{67604B43-B0E8-4EFB-8E4E-E4BE87F04D43}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -127,7 +136,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00049684/detail</t>
       </text>
     </comment>
-    <comment ref="H5" authorId="7" shapeId="0" xr:uid="{CCF7D895-9024-4EB3-B4C8-9D4267AD910D}">
+    <comment ref="H5" authorId="8" shapeId="0" xr:uid="{CCF7D895-9024-4EB3-B4C8-9D4267AD910D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -137,7 +146,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00043875/detail</t>
       </text>
     </comment>
-    <comment ref="H7" authorId="8" shapeId="0" xr:uid="{CCE18EB5-1980-4F82-8A29-0E47102B130E}">
+    <comment ref="H7" authorId="9" shapeId="0" xr:uid="{CCE18EB5-1980-4F82-8A29-0E47102B130E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -147,7 +156,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00041312/detail</t>
       </text>
     </comment>
-    <comment ref="H11" authorId="9" shapeId="0" xr:uid="{6B475501-D57D-4AD6-886C-F6988D084AC9}">
+    <comment ref="H11" authorId="10" shapeId="0" xr:uid="{6B475501-D57D-4AD6-886C-F6988D084AC9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -155,7 +164,7 @@
     Last updated on 7/31/2023; not sure if this is a 4-week delay or this station has been inactivated.</t>
       </text>
     </comment>
-    <comment ref="H13" authorId="10" shapeId="0" xr:uid="{7EE63F13-8F5F-4C5B-9A58-E88B048768BF}">
+    <comment ref="H13" authorId="11" shapeId="0" xr:uid="{7EE63F13-8F5F-4C5B-9A58-E88B048768BF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -165,7 +174,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00043578/detail</t>
       </text>
     </comment>
-    <comment ref="H15" authorId="11" shapeId="0" xr:uid="{50490E16-D2C9-452D-98DD-E34778E8185C}">
+    <comment ref="H15" authorId="12" shapeId="0" xr:uid="{50490E16-D2C9-452D-98DD-E34778E8185C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -175,7 +184,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00046370/detail</t>
       </text>
     </comment>
-    <comment ref="H17" authorId="12" shapeId="0" xr:uid="{EC9754E5-5B68-4A80-A586-4AD6629EAEB7}">
+    <comment ref="H17" authorId="13" shapeId="0" xr:uid="{EC9754E5-5B68-4A80-A586-4AD6629EAEB7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -185,7 +194,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00047109/detail</t>
       </text>
     </comment>
-    <comment ref="H19" authorId="13" shapeId="0" xr:uid="{D8606121-17D8-47A7-B702-46B0EE7C815E}">
+    <comment ref="H19" authorId="14" shapeId="0" xr:uid="{D8606121-17D8-47A7-B702-46B0EE7C815E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -195,7 +204,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00049122/detail</t>
       </text>
     </comment>
-    <comment ref="H23" authorId="14" shapeId="0" xr:uid="{4DC2D99B-876B-4C04-A3D0-3FC8353C2808}">
+    <comment ref="H23" authorId="15" shapeId="0" xr:uid="{4DC2D99B-876B-4C04-A3D0-3FC8353C2808}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -205,7 +214,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00049124/detail</t>
       </text>
     </comment>
-    <comment ref="H29" authorId="15" shapeId="0" xr:uid="{59F2DFAB-28DD-4957-8254-9BCC9173681F}">
+    <comment ref="H29" authorId="16" shapeId="0" xr:uid="{59F2DFAB-28DD-4957-8254-9BCC9173681F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -215,7 +224,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00041838/detail</t>
       </text>
     </comment>
-    <comment ref="H33" authorId="16" shapeId="0" xr:uid="{9E58D42F-FA3B-4C72-AB97-622A776FCDE0}">
+    <comment ref="H33" authorId="17" shapeId="0" xr:uid="{9E58D42F-FA3B-4C72-AB97-622A776FCDE0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -225,7 +234,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00043875/detail</t>
       </text>
     </comment>
-    <comment ref="H35" authorId="17" shapeId="0" xr:uid="{6EFC964B-340F-4EBB-B69B-8D1B880CEF5A}">
+    <comment ref="H35" authorId="18" shapeId="0" xr:uid="{6EFC964B-340F-4EBB-B69B-8D1B880CEF5A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -235,7 +244,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00049122/detail</t>
       </text>
     </comment>
-    <comment ref="H43" authorId="18" shapeId="0" xr:uid="{76278B7B-75A0-4ECB-B25C-ABC7A8820030}">
+    <comment ref="H43" authorId="19" shapeId="0" xr:uid="{76278B7B-75A0-4ECB-B25C-ABC7A8820030}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -245,7 +254,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00047109/detail</t>
       </text>
     </comment>
-    <comment ref="H49" authorId="19" shapeId="0" xr:uid="{09749EE1-E303-4817-845D-F5DE7BCB21D8}">
+    <comment ref="H49" authorId="20" shapeId="0" xr:uid="{09749EE1-E303-4817-845D-F5DE7BCB21D8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -255,7 +264,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00043875/detail</t>
       </text>
     </comment>
-    <comment ref="H51" authorId="20" shapeId="0" xr:uid="{94CCAA68-47B8-484A-BCAD-A61A4E742094}">
+    <comment ref="H51" authorId="21" shapeId="0" xr:uid="{94CCAA68-47B8-484A-BCAD-A61A4E742094}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -265,7 +274,7 @@
     https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND/stations/GHCND:USC00049122/detail</t>
       </text>
     </comment>
-    <comment ref="H59" authorId="21" shapeId="0" xr:uid="{0500963D-B3C2-4267-B108-7DD869A18259}">
+    <comment ref="H59" authorId="22" shapeId="0" xr:uid="{0500963D-B3C2-4267-B108-7DD869A18259}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -280,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="103">
   <si>
     <t>Observed and PRISM Station Guide</t>
   </si>
@@ -321,9 +330,6 @@
     <t>Elevation (ft)</t>
   </si>
   <si>
-    <t>DOWNSIZER</t>
-  </si>
-  <si>
     <t>PRECIP1</t>
   </si>
   <si>
@@ -354,9 +360,6 @@
     <t>PRECIP10</t>
   </si>
   <si>
-    <t>DOWNSIZER_PRECIP10</t>
-  </si>
-  <si>
     <t>HEAC1</t>
   </si>
   <si>
@@ -372,9 +375,6 @@
     <t>PRECIP11</t>
   </si>
   <si>
-    <t>DOWNSIZER_PRECIP11</t>
-  </si>
-  <si>
     <t>RMKC1</t>
   </si>
   <si>
@@ -474,9 +474,6 @@
     <t>PRECIP5</t>
   </si>
   <si>
-    <t>DOWNSIZER_PRECIP5</t>
-  </si>
-  <si>
     <t>USC00049124</t>
   </si>
   <si>
@@ -598,13 +595,16 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>NOAA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,6 +738,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1102,7 +1108,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1120,23 +1126,14 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1367,6 +1364,7 @@
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Alemi, Payman@Waterboards" id="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" userId="S::Payman.Alemi@Waterboards.ca.gov::e620a27f-2ddb-47d8-b6f0-c0d86a0a16eb" providerId="AD"/>
+  <person displayName="Prashar, Aakash@Waterboards" id="{143A89A7-5D5E-42BF-955B-CB49B4CFC167}" userId="S::Aakash.Prashar@Waterboards.ca.gov::8a25d33d-2aea-4ebe-9506-f1c07c221fd4" providerId="AD"/>
 </personList>
 </file>
 
@@ -2102,7 +2100,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="CIMIS" cacheId="2841" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="CIMIS" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
   <location ref="D3:D11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -2224,7 +2222,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12495159-9906-4108-ABA6-894BC3D5D83C}" name="PivotTable3" cacheId="2841" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="CNRFC IDs">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12495159-9906-4108-ABA6-894BC3D5D83C}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="CNRFC IDs">
   <location ref="G1:H15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField multipleItemSelectionAllowed="1" showAll="0">
@@ -2381,7 +2379,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="RAWS" cacheId="2841" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000001000000}" name="RAWS" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Station">
   <location ref="A4:A12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0" defaultSubtotal="0">
@@ -2501,17 +2499,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:L64" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="A2:L64" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="DOWNSIZER"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:L64">
-    <sortCondition ref="B3:B64"/>
-    <sortCondition ref="A3:A64"/>
-  </sortState>
+  <autoFilter ref="A2:L64" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Source" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Rank" dataDxfId="9"/>
@@ -2531,9 +2519,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2571,7 +2559,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2677,7 +2665,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2819,7 +2807,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2833,7 +2821,7 @@
   <threadedComment ref="D2" dT="2022-12-09T00:10:46.39" personId="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" id="{BC7C7AE7-6F87-4221-9502-CF9F5DB40310}">
     <text>CNRFC = California Nevada River Forecast Center; these are the IDs that show up for these stations when you download the 6-day forecast CSV from CNRFC's website</text>
   </threadedComment>
-  <threadedComment ref="E2" dT="2022-12-09T00:11:56.91" personId="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" id="{22596FE2-5E99-4CF2-B004-07E21D8F2E47}">
+  <threadedComment ref="E2" dT="2022-12-09T00:11:56.91" personId="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" id="{22596FE2-5E99-4CF2-B004-07E21D8F2E47}" done="1">
     <text>Downsizer stations have GHCND station IDs while RAWS and CIMIS stations often don't and instead use a different naming convention. GHCND data is provided by NOAA NCDC: https://www.ncdc.noaa.gov/cdo-web/datasets/GHCND.</text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -2865,6 +2853,9 @@
   </threadedComment>
   <threadedComment ref="L2" dT="2023-08-28T19:14:14.77" personId="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" id="{AD3D0412-D381-472E-8164-396C8D02E097}">
     <text>The PRISM stations that are used to fill in the missing data for our weather stations have the same longitude and latitude, but different elevations. Is this an issue?</text>
+  </threadedComment>
+  <threadedComment ref="A3" dT="2024-02-06T20:09:51.64" personId="{143A89A7-5D5E-42BF-955B-CB49B4CFC167}" id="{42A02FD6-F123-4517-A0FF-D7A041A3BB47}">
+    <text xml:space="preserve">NOAA stations were formerly DOWNSIZER stations, but then SDU discovered that the program Downsizer is a GUI for collecting NOAA station data. Hence, we decided to download data from NOAA directly instead. </text>
   </threadedComment>
   <threadedComment ref="H3" dT="2023-08-29T00:47:04.42" personId="{C7A984B0-AAAC-4294-9284-9BB567C9E403}" id="{67604B43-B0E8-4EFB-8E4E-E4BE87F04D43}">
     <text>Last data uploaded to NCDC NOAA on 9/27/2012; replace entirely with PRISM.</text>
@@ -3056,36 +3047,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21" customHeight="1">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -3097,7 +3088,7 @@
       <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -3109,41 +3100,41 @@
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
       </c>
       <c r="C3" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP1</v>
+        <v>NOAA_PRECIP1</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="1">
+        <v>49684</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="9">
-        <v>49684</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>18</v>
       </c>
       <c r="I3" s="1">
         <v>-999</v>
@@ -3158,30 +3149,30 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="J4">
         <v>39.419400000000003</v>
@@ -3190,65 +3181,66 @@
         <v>-123.3425</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
+        <v>NOAA_PRECIP10</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" s="1">
+        <v>43875</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9">
-        <v>43875</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="14">
+      <c r="J5">
         <v>38.629399999999997</v>
       </c>
-      <c r="K5" s="14">
+      <c r="K5">
         <v>-122.8665</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J6">
         <v>38.629399999999997</v>
@@ -3256,35 +3248,35 @@
       <c r="K6">
         <v>-122.8665</v>
       </c>
-      <c r="L6" s="14"/>
-    </row>
-    <row r="7" spans="1:12">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
+        <v>NOAA_PRECIP11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F7" s="1">
+        <v>41312</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="9">
-        <v>41312</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="J7">
         <v>38.5961</v>
@@ -3296,27 +3288,27 @@
         <v>400</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J8">
         <v>38.5961</v>
@@ -3325,28 +3317,28 @@
         <v>-122.60129999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C9" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_PRECIP12</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9">
         <f>38+31/60</f>
@@ -3356,31 +3348,31 @@
         <f>-122-50/60</f>
         <v>-122.83333333333333</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L9" s="11">
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J10" s="6">
         <v>38.526000000000003</v>
@@ -3390,34 +3382,34 @@
       </c>
       <c r="L10" s="6"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP13</v>
+        <v>NOAA_PRECIP13</v>
       </c>
       <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="1">
+        <v>43191</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="9">
-        <v>43191</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>42</v>
-      </c>
       <c r="I11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11">
         <v>38.515000000000001</v>
@@ -3429,27 +3421,27 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J12">
         <v>38.515000000000001</v>
@@ -3458,34 +3450,34 @@
         <v>-123.24469999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP14</v>
+        <v>NOAA_PRECIP14</v>
       </c>
       <c r="D13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="9">
+        <v>41</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="1">
         <v>43578</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>42</v>
+      <c r="G13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="6">
         <v>38.430500000000002</v>
@@ -3497,27 +3489,27 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J14">
         <v>38.430500000000002</v>
@@ -3526,31 +3518,31 @@
         <v>-122.8647</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP15</v>
+        <v>NOAA_PRECIP15</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="9">
+        <v>36</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="1">
         <v>46370</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>18</v>
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I15" s="1">
         <v>-999</v>
@@ -3565,27 +3557,27 @@
         <v>865</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J16">
         <v>38.385800000000003</v>
@@ -3594,66 +3586,66 @@
         <v>-122.9661</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C17" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP2</v>
+        <v>NOAA_PRECIP2</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="9">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="1">
         <v>47109</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>21</v>
+      <c r="G17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="14">
+        <v>26</v>
+      </c>
+      <c r="J17">
         <v>39.361899999999999</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17">
         <v>-123.12860000000001</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17">
         <v>1018</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J18">
         <v>39.361899999999999</v>
@@ -3662,31 +3654,31 @@
         <v>-123.12860000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C19" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP3</v>
+        <v>NOAA_PRECIP3</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="9">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="1">
         <v>49122</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>18</v>
+      <c r="G19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I19" s="1">
         <v>-999</v>
@@ -3701,27 +3693,27 @@
         <v>636</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J20">
         <v>39.146599999999999</v>
@@ -3730,27 +3722,27 @@
         <v>-123.2102</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J21">
         <v>39.125799999999998</v>
@@ -3759,62 +3751,63 @@
         <v>-123.0736</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>60</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>61</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J22" s="13">
+        <v>26</v>
+      </c>
+      <c r="J22" s="10">
         <v>39.125799999999998</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="10">
         <v>-123.0736</v>
       </c>
-      <c r="L22" s="16" t="s">
+      <c r="L22" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
+        <v>NOAA_PRECIP5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" s="1">
+        <v>49124</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="9">
-        <v>49124</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>18</v>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I23" s="1">
         <v>-999</v>
@@ -3829,27 +3822,27 @@
         <v>1328</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J24">
         <v>39.126600000000003</v>
@@ -3858,62 +3851,62 @@
         <v>-123.2719</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C25" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_PRECIP6</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>68</v>
+        <v>57</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="9" t="s">
-        <v>18</v>
+      <c r="H25" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I25" s="1">
         <v>-999</v>
       </c>
-      <c r="J25" s="14">
+      <c r="J25">
         <v>39.030833000000001</v>
       </c>
-      <c r="K25" s="14">
+      <c r="K25">
         <v>-123.080556</v>
       </c>
-      <c r="L25" s="17">
+      <c r="L25" s="11">
         <v>2682</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J26">
         <v>39.006700000000002</v>
@@ -3923,27 +3916,27 @@
       </c>
       <c r="L26" s="6"/>
     </row>
-    <row r="27" spans="1:12" hidden="1">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E27" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J27">
         <v>38.987499999999997</v>
@@ -3952,99 +3945,99 @@
         <v>-123.3486</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C28" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_PRECIP7</v>
       </c>
       <c r="D28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J28" s="14">
+        <v>21</v>
+      </c>
+      <c r="J28">
         <v>39.987499999999997</v>
       </c>
-      <c r="K28" s="14">
+      <c r="K28">
         <v>-123.34861100000001</v>
       </c>
-      <c r="L28" s="17">
+      <c r="L28" s="11">
         <v>644</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C29" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_PRECIP8</v>
+        <v>NOAA_PRECIP8</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="9">
+        <v>69</v>
+      </c>
+      <c r="F29" s="1">
         <v>41838</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H29" s="9" t="s">
+      <c r="G29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J29" s="14">
+      <c r="J29">
         <v>38.792999999999999</v>
       </c>
-      <c r="K29" s="14">
+      <c r="K29">
         <v>-123.02630000000001</v>
       </c>
-      <c r="L29" s="14">
+      <c r="L29">
         <v>400</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J30">
         <v>38.792999999999999</v>
@@ -4053,27 +4046,27 @@
         <v>-123.02630000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J31">
         <v>38.781700000000001</v>
@@ -4082,99 +4075,99 @@
         <v>-122.9169</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C32" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_PRECIP9</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J32" s="13">
+        <v>26</v>
+      </c>
+      <c r="J32" s="10">
         <v>38.781700000000001</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K32" s="10">
         <v>-122.9169</v>
       </c>
-      <c r="L32" s="16">
+      <c r="L32" s="12">
         <v>609.6</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C33" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMAX1</v>
+        <v>NOAA_TMAX1</v>
       </c>
       <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="1">
+        <v>43875</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E33" t="s">
+      <c r="H33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="9">
-        <v>43875</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J33" s="14">
+      <c r="J33">
         <v>38.629399999999997</v>
       </c>
-      <c r="K33" s="14">
+      <c r="K33">
         <v>-122.8665</v>
       </c>
-      <c r="L33" s="14">
+      <c r="L33">
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:12" hidden="1">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J34">
         <v>38.629399999999997</v>
@@ -4183,31 +4176,31 @@
         <v>-122.8665</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C35" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMAX2</v>
+        <v>NOAA_TMAX2</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" t="s">
-        <v>55</v>
-      </c>
-      <c r="F35" s="9">
+        <v>52</v>
+      </c>
+      <c r="F35" s="1">
         <v>49122</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>18</v>
+      <c r="G35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I35" s="1">
         <v>-999</v>
@@ -4222,27 +4215,27 @@
         <v>636</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
+        <v>19</v>
+      </c>
+      <c r="E36" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J36">
         <v>39.146700000000003</v>
@@ -4251,28 +4244,28 @@
         <v>-123.2103</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C37" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_TMAX3</v>
       </c>
       <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J37">
         <v>39.146599999999999</v>
@@ -4281,27 +4274,27 @@
         <v>-123.2102</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J38">
         <v>38.982999999999997</v>
@@ -4310,28 +4303,28 @@
         <v>-123.092</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C39" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_TMAX4</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>85</v>
+        <v>41</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J39">
         <v>38.401001000000001</v>
@@ -4340,27 +4333,27 @@
         <v>-122.795998</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J40">
         <v>38.401000000000003</v>
@@ -4369,27 +4362,27 @@
         <v>-122.79600000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E41" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J41">
         <v>38.781700000000001</v>
@@ -4398,67 +4391,67 @@
         <v>-122.9169</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C42" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMAX5</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J42" s="13">
+        <v>26</v>
+      </c>
+      <c r="J42" s="10">
         <v>38.781700000000001</v>
       </c>
-      <c r="K42" s="13">
+      <c r="K42" s="10">
         <v>-122.9169</v>
       </c>
-      <c r="L42" s="16">
+      <c r="L42" s="12">
         <v>609.6</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C43" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMAX6</v>
+        <v>NOAA_TMAX6</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" s="9">
+        <v>49</v>
+      </c>
+      <c r="F43" s="1">
         <v>47109</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>21</v>
+      <c r="G43" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J43">
         <v>39.361899999999999</v>
@@ -4470,27 +4463,27 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E44" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J44">
         <v>39.361899999999999</v>
@@ -4499,27 +4492,27 @@
         <v>-123.12860000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J45">
         <v>39.125799999999998</v>
@@ -4528,60 +4521,60 @@
         <v>-123.0736</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C46" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMAX7</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>61</v>
+        <v>86</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J46" s="13">
+        <v>26</v>
+      </c>
+      <c r="J46" s="10">
         <v>39.125799999999998</v>
       </c>
-      <c r="K46" s="13">
+      <c r="K46" s="10">
         <v>-123.0736</v>
       </c>
-      <c r="L46" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" hidden="1">
+      <c r="L46" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J47">
         <v>38.4786</v>
@@ -4590,28 +4583,28 @@
         <v>-122.81189999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" hidden="1">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C48" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMAX8</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
-      </c>
-      <c r="E48" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J48">
         <v>38.478611110000003</v>
@@ -4623,66 +4616,66 @@
         <v>576</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C49" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMIN1</v>
+        <v>NOAA_TMIN1</v>
       </c>
       <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="1">
+        <v>43875</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E49" t="s">
+      <c r="H49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="9">
-        <v>43875</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J49" s="14">
+      <c r="J49">
         <v>38.629399999999997</v>
       </c>
-      <c r="K49" s="14">
+      <c r="K49">
         <v>-122.8665</v>
       </c>
-      <c r="L49" s="14">
+      <c r="L49">
         <v>177</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G50" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J50">
         <v>38.629399999999997</v>
@@ -4692,31 +4685,31 @@
       </c>
       <c r="L50" s="6"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C51" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMIN2</v>
+        <v>NOAA_TMIN2</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F51" s="9">
+        <v>52</v>
+      </c>
+      <c r="F51" s="1">
         <v>49122</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>18</v>
+      <c r="G51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="I51" s="1">
         <v>-999</v>
@@ -4731,27 +4724,27 @@
         <v>636</v>
       </c>
     </row>
-    <row r="52" spans="1:12" hidden="1">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J52">
         <v>39.146700000000003</v>
@@ -4760,28 +4753,28 @@
         <v>-123.2103</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C53" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_TMIN3</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>82</v>
+        <v>68</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J53">
         <v>39.146599999999999</v>
@@ -4790,27 +4783,27 @@
         <v>-123.2102</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H54" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G54" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J54">
         <v>38.982999999999997</v>
@@ -4818,30 +4811,29 @@
       <c r="K54">
         <v>-123.092</v>
       </c>
-      <c r="L54" s="14"/>
-    </row>
-    <row r="55" spans="1:12" hidden="1">
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C55" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>CIMIS_TMIN4</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>85</v>
+        <v>41</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J55">
         <v>38.401001000000001</v>
@@ -4850,27 +4842,27 @@
         <v>-122.795998</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D56" t="s">
+        <v>19</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J56">
         <v>38.401000000000003</v>
@@ -4878,29 +4870,28 @@
       <c r="K56">
         <v>-122.79600000000001</v>
       </c>
-      <c r="L56" s="14"/>
-    </row>
-    <row r="57" spans="1:12" hidden="1">
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J57">
         <v>38.781700000000001</v>
@@ -4909,28 +4900,28 @@
         <v>-122.9169</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C58" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMIN5</v>
       </c>
       <c r="D58" t="s">
-        <v>87</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J58" s="7">
         <v>38.781700000000001</v>
@@ -4942,66 +4933,66 @@
         <v>609.6</v>
       </c>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C59" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
-        <v>DOWNSIZER_TMIN6</v>
+        <v>NOAA_TMIN6</v>
       </c>
       <c r="D59" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E59" t="s">
-        <v>52</v>
-      </c>
-      <c r="F59" s="9">
+        <v>49</v>
+      </c>
+      <c r="F59" s="1">
         <v>47109</v>
       </c>
-      <c r="G59" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H59" s="9" t="s">
-        <v>21</v>
+      <c r="G59" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J59" s="14">
+        <v>26</v>
+      </c>
+      <c r="J59">
         <v>39.361899999999999</v>
       </c>
-      <c r="K59" s="14">
+      <c r="K59">
         <v>-123.12860000000001</v>
       </c>
-      <c r="L59" s="14">
+      <c r="L59">
         <v>1018</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H60" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J60">
         <v>39.361899999999999</v>
@@ -5010,27 +5001,27 @@
         <v>-123.12860000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B61" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G61" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H61" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J61">
         <v>39.125799999999998</v>
@@ -5039,60 +5030,60 @@
         <v>-123.0736</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B62" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C62" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMIN7</v>
       </c>
       <c r="D62" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>61</v>
+        <v>86</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J62" s="13">
+        <v>26</v>
+      </c>
+      <c r="J62" s="10">
         <v>39.125799999999998</v>
       </c>
-      <c r="K62" s="13">
+      <c r="K62" s="10">
         <v>-123.0736</v>
       </c>
-      <c r="L62" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" hidden="1">
+      <c r="L62" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D63" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G63" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="H63" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="J63">
         <v>38.4786</v>
@@ -5101,28 +5092,28 @@
         <v>-122.81189999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:12" hidden="1">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B64" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C64" t="str">
         <f>_xlfn.CONCAT(Table1[[#This Row],[Source]], "_",Table1[[#This Row],[Rank]])</f>
         <v>RAWS_TMIN8</v>
       </c>
       <c r="D64" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J64" s="6">
         <v>38.478611110000003</v>
@@ -5134,7 +5125,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="5"/>
     </row>
   </sheetData>
@@ -5155,256 +5146,256 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="9" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="53" max="54" width="8" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="56" max="57" width="8" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="8" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="8" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="63" max="64" width="8" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="66" max="67" width="8" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="69" max="70" width="8" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="18"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D3" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H3">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4">
         <v>-999</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G13" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="G15" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H15">
         <v>31</v>
@@ -5420,6 +5411,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F312EB754F236045A0D3EDD082CC91AE" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="82994dfdf4a06edb93720da2ee47aef0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06" xmlns:ns3="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8935436539ef92ddb38fac9e2b6a7f63" ns2:_="" ns3:_="">
     <xsd:import namespace="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
@@ -5648,19 +5648,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2381C67C-FB5D-4D2C-A4ED-D13D18DBD961}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEC31F2C-BA94-4757-B459-232C7EAF18FB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2381C67C-FB5D-4D2C-A4ED-D13D18DBD961}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2cf8adb-cf25-47fc-8c92-b53f2a7e7f06"/>
+    <ds:schemaRef ds:uri="851dfaa3-aae8-4c03-b90c-7dd4a6526d0d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>